<commit_message>
Updated functions and tests
</commit_message>
<xml_diff>
--- a/config/SetTestCase/SetTestCases.xlsx
+++ b/config/SetTestCase/SetTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14910" windowHeight="7275"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14910" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -27,9 +27,6 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>testSubscribe</t>
-  </si>
-  <si>
     <t>testBlogs</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>testWorkFrontJobs</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,10 +402,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -413,10 +413,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>